<commit_message>
Falta so o relatorio a mao e mandar o email para o professor
</commit_message>
<xml_diff>
--- a/Arquivos/Portugol-Autoavaliacao.xlsx
+++ b/Arquivos/Portugol-Autoavaliacao.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UESC\Cursos e Disciplinas\Compiladores\Compiladores 2017.2\3- Avaliações\1- Av 1a - Análise Léxica - 1a Chamada\04- Entregue a alunos\Compiladores-2017-2-Credito-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eberty\Dropbox\DocumentosCIC\Semestre6\Compiladores\ProjetoCompiladoresEbertyPhiliphe\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="160" windowWidth="11520" windowHeight="9520" tabRatio="393"/>
+    <workbookView xWindow="-24" yWindow="156" windowWidth="11520" windowHeight="9516" tabRatio="393" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Critérios" sheetId="105" r:id="rId1"/>
@@ -1840,6 +1840,171 @@
     <xf numFmtId="168" fontId="7" fillId="14" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="64" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="68" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="68" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="70" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="70" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="74" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="74" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1858,6 +2023,57 @@
     <xf numFmtId="0" fontId="28" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="31" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="31" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="31" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="40" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="40" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="40" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="22" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1867,57 +2083,6 @@
     <xf numFmtId="0" fontId="29" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="31" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="31" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="31" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="40" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="40" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="40" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="22" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="166" fontId="30" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2028,177 +2193,12 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="24" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="64" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="68" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="68" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="70" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="70" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="74" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="74" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -2639,7 +2639,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2961,596 +2961,596 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="213" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" style="214" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" style="215" customWidth="1"/>
-    <col min="4" max="4" width="4.26953125" style="216" customWidth="1"/>
-    <col min="5" max="5" width="58" style="215" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.26953125" style="217" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="194"/>
+    <col min="1" max="1" width="4" style="126" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="127" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" style="128" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" style="129" customWidth="1"/>
+    <col min="5" max="5" width="58" style="128" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.21875" style="130" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.21875" style="119"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="167" customFormat="1" ht="31">
-      <c r="A1" s="163" t="s">
+    <row r="1" spans="1:9" s="101" customFormat="1" ht="31.2">
+      <c r="A1" s="131" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-    </row>
-    <row r="2" spans="1:9" s="172" customFormat="1" ht="26">
-      <c r="A2" s="168" t="s">
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+    </row>
+    <row r="2" spans="1:9" s="103" customFormat="1" ht="25.8">
+      <c r="A2" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
-      <c r="I2" s="171"/>
-    </row>
-    <row r="3" spans="1:9" s="172" customFormat="1" ht="23.5">
-      <c r="A3" s="173" t="s">
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+    </row>
+    <row r="3" spans="1:9" s="103" customFormat="1" ht="23.4">
+      <c r="A3" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-    </row>
-    <row r="4" spans="1:9" s="167" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="177"/>
-      <c r="B4" s="178"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="179"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-    </row>
-    <row r="5" spans="1:9" s="187" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A5" s="182"/>
-      <c r="B5" s="183" t="s">
+      <c r="B3" s="138"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+    </row>
+    <row r="4" spans="1:9" s="101" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="105"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+    </row>
+    <row r="5" spans="1:9" s="115" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A5" s="110"/>
+      <c r="B5" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="184" t="s">
+      <c r="C5" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="185" t="s">
+      <c r="D5" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="184" t="s">
+      <c r="E5" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="186" t="s">
+      <c r="F5" s="114" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A6" s="188" t="s">
+    <row r="6" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A6" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="189">
+      <c r="B6" s="143">
         <v>2</v>
       </c>
-      <c r="C6" s="190" t="s">
+      <c r="C6" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="191">
+      <c r="D6" s="116">
         <v>1</v>
       </c>
-      <c r="E6" s="192" t="s">
+      <c r="E6" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="193">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A7" s="188"/>
-      <c r="B7" s="195"/>
-      <c r="C7" s="196"/>
-      <c r="D7" s="191">
+      <c r="F6" s="118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A7" s="142"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="116">
         <f t="shared" ref="D7:D13" si="0">D6+1</f>
         <v>2</v>
       </c>
-      <c r="E7" s="192" t="s">
+      <c r="E7" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="193">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A8" s="188"/>
-      <c r="B8" s="195"/>
-      <c r="C8" s="196"/>
-      <c r="D8" s="191">
+      <c r="F7" s="118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A8" s="142"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="116">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E8" s="192" t="s">
+      <c r="E8" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="193">
+      <c r="F8" s="118">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A9" s="188"/>
-      <c r="B9" s="197"/>
-      <c r="C9" s="198"/>
-      <c r="D9" s="191">
+    <row r="9" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A9" s="142"/>
+      <c r="B9" s="145"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="116">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E9" s="192" t="s">
+      <c r="E9" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="193">
+      <c r="F9" s="118">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A10" s="188"/>
-      <c r="B10" s="189">
+    <row r="10" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A10" s="142"/>
+      <c r="B10" s="143">
         <v>2</v>
       </c>
-      <c r="C10" s="190" t="s">
+      <c r="C10" s="146" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="191">
+      <c r="D10" s="116">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E10" s="192" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="193">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A11" s="188"/>
-      <c r="B11" s="195"/>
-      <c r="C11" s="196"/>
-      <c r="D11" s="191">
+      <c r="E10" s="117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A11" s="142"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="147"/>
+      <c r="D11" s="116">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E11" s="192" t="s">
+      <c r="E11" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="193">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A12" s="188"/>
-      <c r="B12" s="195"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="191">
+      <c r="F11" s="118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A12" s="142"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="116">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E12" s="192" t="s">
+      <c r="E12" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="193">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A13" s="188"/>
-      <c r="B13" s="195"/>
-      <c r="C13" s="196"/>
-      <c r="D13" s="191">
+      <c r="F12" s="118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A13" s="142"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="116">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E13" s="192" t="s">
+      <c r="E13" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="193">
+      <c r="F13" s="118">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A14" s="188"/>
-      <c r="B14" s="197"/>
-      <c r="C14" s="198"/>
-      <c r="D14" s="191">
+    <row r="14" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A14" s="142"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="116">
         <f t="shared" ref="D14:D29" si="1">D13+1</f>
         <v>9</v>
       </c>
-      <c r="E14" s="192" t="s">
+      <c r="E14" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="193">
+      <c r="F14" s="118">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A15" s="199" t="s">
+    <row r="15" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A15" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="200">
+      <c r="B15" s="140">
         <v>4</v>
       </c>
-      <c r="C15" s="201" t="s">
+      <c r="C15" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="202">
+      <c r="D15" s="120">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E15" s="203" t="s">
+      <c r="E15" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="204">
+      <c r="F15" s="122">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="13.25" customHeight="1">
-      <c r="A16" s="199"/>
-      <c r="B16" s="200"/>
-      <c r="C16" s="201"/>
-      <c r="D16" s="202">
+    <row r="16" spans="1:9" ht="13.2" customHeight="1">
+      <c r="A16" s="149"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="120">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="E16" s="203" t="s">
+      <c r="E16" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="204">
+      <c r="F16" s="122">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A17" s="199"/>
-      <c r="B17" s="200"/>
-      <c r="C17" s="201"/>
-      <c r="D17" s="202">
+    <row r="17" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A17" s="149"/>
+      <c r="B17" s="140"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="120">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="E17" s="203" t="s">
+      <c r="E17" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="204">
+      <c r="F17" s="122">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A18" s="199"/>
-      <c r="B18" s="200">
+    <row r="18" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A18" s="149"/>
+      <c r="B18" s="140">
         <v>3</v>
       </c>
-      <c r="C18" s="201" t="s">
+      <c r="C18" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="202">
+      <c r="D18" s="120">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E18" s="203" t="s">
+      <c r="E18" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="204">
+      <c r="F18" s="122">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A19" s="199"/>
-      <c r="B19" s="200"/>
-      <c r="C19" s="201"/>
-      <c r="D19" s="202">
+    <row r="19" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A19" s="149"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="120">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="E19" s="203" t="s">
+      <c r="E19" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="204">
+      <c r="F19" s="122">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A20" s="199"/>
-      <c r="B20" s="200">
+    <row r="20" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A20" s="149"/>
+      <c r="B20" s="140">
         <v>4</v>
       </c>
-      <c r="C20" s="201" t="s">
+      <c r="C20" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="202">
+      <c r="D20" s="120">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E20" s="203" t="s">
+      <c r="E20" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="204">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A21" s="199"/>
-      <c r="B21" s="200"/>
-      <c r="C21" s="201"/>
-      <c r="D21" s="202">
+      <c r="F20" s="122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A21" s="149"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="120">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="E21" s="203" t="s">
+      <c r="E21" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="204">
+      <c r="F21" s="122">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A22" s="199"/>
-      <c r="B22" s="200"/>
-      <c r="C22" s="201"/>
-      <c r="D22" s="202">
+    <row r="22" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A22" s="149"/>
+      <c r="B22" s="140"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="120">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="E22" s="203" t="s">
+      <c r="E22" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="204">
+      <c r="F22" s="122">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A23" s="199"/>
-      <c r="B23" s="200">
+    <row r="23" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A23" s="149"/>
+      <c r="B23" s="140">
         <v>4</v>
       </c>
-      <c r="C23" s="201" t="s">
+      <c r="C23" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="202">
+      <c r="D23" s="120">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="E23" s="203" t="s">
+      <c r="E23" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="204">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A24" s="199"/>
-      <c r="B24" s="200"/>
-      <c r="C24" s="201"/>
-      <c r="D24" s="202">
+      <c r="F23" s="122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A24" s="149"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="120">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E24" s="203" t="s">
+      <c r="E24" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="204">
+      <c r="F24" s="122">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A25" s="199"/>
-      <c r="B25" s="200"/>
-      <c r="C25" s="201"/>
-      <c r="D25" s="202">
+    <row r="25" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A25" s="149"/>
+      <c r="B25" s="140"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="120">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="E25" s="203" t="s">
+      <c r="E25" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="204">
+      <c r="F25" s="122">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A26" s="199"/>
-      <c r="B26" s="200">
+    <row r="26" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A26" s="149"/>
+      <c r="B26" s="140">
         <v>3</v>
       </c>
-      <c r="C26" s="201" t="s">
+      <c r="C26" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="202">
+      <c r="D26" s="120">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="E26" s="203" t="s">
+      <c r="E26" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="204">
+      <c r="F26" s="122">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A27" s="199"/>
-      <c r="B27" s="200"/>
-      <c r="C27" s="201"/>
-      <c r="D27" s="202">
+    <row r="27" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A27" s="149"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="120">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="E27" s="203" t="s">
+      <c r="E27" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="204">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A28" s="205" t="s">
+      <c r="F27" s="122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A28" s="150" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="206">
+      <c r="B28" s="153">
         <v>3</v>
       </c>
-      <c r="C28" s="207" t="s">
+      <c r="C28" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="208">
+      <c r="D28" s="123">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="E28" s="209" t="s">
+      <c r="E28" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="210">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A29" s="211"/>
-      <c r="B29" s="206"/>
-      <c r="C29" s="207"/>
-      <c r="D29" s="208">
+      <c r="F28" s="125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A29" s="151"/>
+      <c r="B29" s="153"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="123">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="E29" s="209" t="s">
+      <c r="E29" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="210">
+      <c r="F29" s="125">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A30" s="211"/>
-      <c r="B30" s="206"/>
-      <c r="C30" s="207"/>
-      <c r="D30" s="208">
+    <row r="30" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A30" s="151"/>
+      <c r="B30" s="153"/>
+      <c r="C30" s="154"/>
+      <c r="D30" s="123">
         <f t="shared" ref="D30:D36" si="2">D29+1</f>
         <v>25</v>
       </c>
-      <c r="E30" s="209" t="s">
+      <c r="E30" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="210">
+      <c r="F30" s="125">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A31" s="211"/>
-      <c r="B31" s="206">
+    <row r="31" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A31" s="151"/>
+      <c r="B31" s="153">
         <v>3</v>
       </c>
-      <c r="C31" s="207" t="s">
+      <c r="C31" s="154" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="208">
+      <c r="D31" s="123">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="E31" s="209" t="s">
+      <c r="E31" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="210">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A32" s="211"/>
-      <c r="B32" s="206"/>
-      <c r="C32" s="207"/>
-      <c r="D32" s="208">
+      <c r="F31" s="125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A32" s="151"/>
+      <c r="B32" s="153"/>
+      <c r="C32" s="154"/>
+      <c r="D32" s="123">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="E32" s="209" t="s">
+      <c r="E32" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="210">
+      <c r="F32" s="125">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A33" s="211"/>
-      <c r="B33" s="206"/>
-      <c r="C33" s="207"/>
-      <c r="D33" s="208">
+    <row r="33" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A33" s="151"/>
+      <c r="B33" s="153"/>
+      <c r="C33" s="154"/>
+      <c r="D33" s="123">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="E33" s="209" t="s">
+      <c r="E33" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="210">
+      <c r="F33" s="125">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A34" s="211"/>
-      <c r="B34" s="206">
+    <row r="34" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A34" s="151"/>
+      <c r="B34" s="153">
         <v>3</v>
       </c>
-      <c r="C34" s="207" t="s">
+      <c r="C34" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="208">
+      <c r="D34" s="123">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="E34" s="209" t="s">
+      <c r="E34" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="210">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A35" s="211"/>
-      <c r="B35" s="206"/>
-      <c r="C35" s="207"/>
-      <c r="D35" s="208">
+      <c r="F34" s="125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A35" s="151"/>
+      <c r="B35" s="153"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="123">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="E35" s="209" t="s">
+      <c r="E35" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="210">
+      <c r="F35" s="125">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A36" s="212"/>
-      <c r="B36" s="206"/>
-      <c r="C36" s="207"/>
-      <c r="D36" s="208">
+    <row r="36" spans="1:6" ht="13.2" customHeight="1">
+      <c r="A36" s="152"/>
+      <c r="B36" s="153"/>
+      <c r="C36" s="154"/>
+      <c r="D36" s="123">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="E36" s="209" t="s">
+      <c r="E36" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="210">
+      <c r="F36" s="125">
         <v>3</v>
       </c>
     </row>
@@ -3597,134 +3597,134 @@
   </sheetPr>
   <dimension ref="A1:AH16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="47" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" style="46" customWidth="1"/>
-    <col min="3" max="3" width="0.81640625" style="47" customWidth="1"/>
-    <col min="4" max="34" width="3.26953125" style="46" customWidth="1"/>
-    <col min="35" max="16384" width="9.1796875" style="46"/>
+    <col min="1" max="1" width="2.77734375" style="47" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="46" customWidth="1"/>
+    <col min="3" max="3" width="0.77734375" style="47" customWidth="1"/>
+    <col min="4" max="34" width="3.21875" style="46" customWidth="1"/>
+    <col min="35" max="16384" width="9.21875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="31">
-      <c r="A1" s="100" t="str">
+    <row r="1" spans="1:34" ht="31.2">
+      <c r="A1" s="155" t="str">
         <f>Critérios!A1</f>
         <v>Compiladores - 2017.2</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
-      <c r="AA1" s="101"/>
-      <c r="AB1" s="101"/>
-      <c r="AC1" s="101"/>
-      <c r="AD1" s="101"/>
-      <c r="AE1" s="101"/>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="101"/>
-      <c r="AH1" s="102"/>
-    </row>
-    <row r="2" spans="1:34" ht="26">
-      <c r="A2" s="103" t="str">
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="156"/>
+      <c r="L1" s="156"/>
+      <c r="M1" s="156"/>
+      <c r="N1" s="156"/>
+      <c r="O1" s="156"/>
+      <c r="P1" s="156"/>
+      <c r="Q1" s="156"/>
+      <c r="R1" s="156"/>
+      <c r="S1" s="156"/>
+      <c r="T1" s="156"/>
+      <c r="U1" s="156"/>
+      <c r="V1" s="156"/>
+      <c r="W1" s="156"/>
+      <c r="X1" s="156"/>
+      <c r="Y1" s="156"/>
+      <c r="Z1" s="156"/>
+      <c r="AA1" s="156"/>
+      <c r="AB1" s="156"/>
+      <c r="AC1" s="156"/>
+      <c r="AD1" s="156"/>
+      <c r="AE1" s="156"/>
+      <c r="AF1" s="156"/>
+      <c r="AG1" s="156"/>
+      <c r="AH1" s="157"/>
+    </row>
+    <row r="2" spans="1:34" ht="25.8">
+      <c r="A2" s="158" t="str">
         <f>Critérios!A2</f>
         <v xml:space="preserve">Curso: Ciência da Computação </v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="104"/>
-      <c r="AC2" s="104"/>
-      <c r="AD2" s="104"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="104"/>
-      <c r="AH2" s="105"/>
-    </row>
-    <row r="3" spans="1:34" s="47" customFormat="1" ht="23.5">
-      <c r="A3" s="106" t="s">
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="159"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="159"/>
+      <c r="S2" s="159"/>
+      <c r="T2" s="159"/>
+      <c r="U2" s="159"/>
+      <c r="V2" s="159"/>
+      <c r="W2" s="159"/>
+      <c r="X2" s="159"/>
+      <c r="Y2" s="159"/>
+      <c r="Z2" s="159"/>
+      <c r="AA2" s="159"/>
+      <c r="AB2" s="159"/>
+      <c r="AC2" s="159"/>
+      <c r="AD2" s="159"/>
+      <c r="AE2" s="159"/>
+      <c r="AF2" s="159"/>
+      <c r="AG2" s="159"/>
+      <c r="AH2" s="160"/>
+    </row>
+    <row r="3" spans="1:34" s="47" customFormat="1" ht="23.4">
+      <c r="A3" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
-      <c r="AB3" s="107"/>
-      <c r="AC3" s="107"/>
-      <c r="AD3" s="107"/>
-      <c r="AE3" s="107"/>
-      <c r="AF3" s="107"/>
-      <c r="AG3" s="107"/>
-      <c r="AH3" s="108"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
+      <c r="P3" s="179"/>
+      <c r="Q3" s="179"/>
+      <c r="R3" s="179"/>
+      <c r="S3" s="179"/>
+      <c r="T3" s="179"/>
+      <c r="U3" s="179"/>
+      <c r="V3" s="179"/>
+      <c r="W3" s="179"/>
+      <c r="X3" s="179"/>
+      <c r="Y3" s="179"/>
+      <c r="Z3" s="179"/>
+      <c r="AA3" s="179"/>
+      <c r="AB3" s="179"/>
+      <c r="AC3" s="179"/>
+      <c r="AD3" s="179"/>
+      <c r="AE3" s="179"/>
+      <c r="AF3" s="179"/>
+      <c r="AG3" s="179"/>
+      <c r="AH3" s="180"/>
     </row>
     <row r="4" spans="1:34" ht="10.5" customHeight="1">
       <c r="A4" s="48"/>
@@ -3739,79 +3739,79 @@
       <c r="J4" s="48"/>
       <c r="K4" s="48"/>
       <c r="L4" s="48"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="112"/>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="112"/>
-      <c r="AF4" s="112"/>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="164"/>
+      <c r="R4" s="164"/>
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="164"/>
+      <c r="Y4" s="164"/>
+      <c r="Z4" s="164"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="164"/>
+      <c r="AC4" s="164"/>
+      <c r="AD4" s="164"/>
+      <c r="AE4" s="164"/>
+      <c r="AF4" s="164"/>
+      <c r="AG4" s="164"/>
+      <c r="AH4" s="164"/>
     </row>
     <row r="5" spans="1:34" ht="17.25" customHeight="1">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="114"/>
+      <c r="B5" s="166"/>
       <c r="C5" s="49"/>
-      <c r="D5" s="119" t="str">
+      <c r="D5" s="171" t="str">
         <f>Critérios!A6</f>
         <v>Autômato</v>
       </c>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="129" t="str">
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
+      <c r="L5" s="171"/>
+      <c r="M5" s="184" t="str">
         <f>Critérios!A15</f>
         <v>Implementação</v>
       </c>
-      <c r="N5" s="129"/>
-      <c r="O5" s="129"/>
-      <c r="P5" s="129"/>
-      <c r="Q5" s="129"/>
-      <c r="R5" s="129"/>
-      <c r="S5" s="129"/>
-      <c r="T5" s="129"/>
-      <c r="U5" s="129"/>
-      <c r="V5" s="129"/>
-      <c r="W5" s="129"/>
-      <c r="X5" s="129"/>
-      <c r="Y5" s="129"/>
-      <c r="Z5" s="130" t="str">
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="184"/>
+      <c r="R5" s="184"/>
+      <c r="S5" s="184"/>
+      <c r="T5" s="184"/>
+      <c r="U5" s="184"/>
+      <c r="V5" s="184"/>
+      <c r="W5" s="184"/>
+      <c r="X5" s="184"/>
+      <c r="Y5" s="184"/>
+      <c r="Z5" s="185" t="str">
         <f>Critérios!A28</f>
         <v>Saídas</v>
       </c>
-      <c r="AA5" s="130"/>
-      <c r="AB5" s="130"/>
-      <c r="AC5" s="130"/>
-      <c r="AD5" s="130"/>
-      <c r="AE5" s="130"/>
-      <c r="AF5" s="130"/>
-      <c r="AG5" s="130"/>
-      <c r="AH5" s="130"/>
+      <c r="AA5" s="185"/>
+      <c r="AB5" s="185"/>
+      <c r="AC5" s="185"/>
+      <c r="AD5" s="185"/>
+      <c r="AE5" s="185"/>
+      <c r="AF5" s="185"/>
+      <c r="AG5" s="185"/>
+      <c r="AH5" s="185"/>
     </row>
     <row r="6" spans="1:34" ht="3.75" customHeight="1">
-      <c r="A6" s="115"/>
-      <c r="B6" s="116"/>
+      <c r="A6" s="167"/>
+      <c r="B6" s="168"/>
       <c r="C6" s="49"/>
       <c r="D6" s="50"/>
       <c r="E6" s="51"/>
@@ -3845,71 +3845,71 @@
       <c r="AG6" s="57"/>
       <c r="AH6" s="58"/>
     </row>
-    <row r="7" spans="1:34" s="60" customFormat="1" ht="113" customHeight="1">
-      <c r="A7" s="117"/>
-      <c r="B7" s="118"/>
+    <row r="7" spans="1:34" s="60" customFormat="1" ht="112.95" customHeight="1">
+      <c r="A7" s="169"/>
+      <c r="B7" s="170"/>
       <c r="C7" s="59"/>
-      <c r="D7" s="126" t="str">
+      <c r="D7" s="181" t="str">
         <f>Critérios!C6</f>
         <v>Diagrama de transições (imagem)</v>
       </c>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="126" t="str">
+      <c r="E7" s="182"/>
+      <c r="F7" s="182"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="181" t="str">
         <f>Critérios!C10</f>
         <v>Tabela de transições (imagem)</v>
       </c>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="109" t="str">
+      <c r="I7" s="182"/>
+      <c r="J7" s="182"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="182"/>
+      <c r="M7" s="161" t="str">
         <f>Critérios!C15</f>
         <v>Tokens</v>
       </c>
-      <c r="N7" s="110"/>
-      <c r="O7" s="111"/>
-      <c r="P7" s="109" t="str">
+      <c r="N7" s="162"/>
+      <c r="O7" s="163"/>
+      <c r="P7" s="161" t="str">
         <f>Critérios!C18</f>
         <v>Palavras reservadas</v>
       </c>
-      <c r="Q7" s="111"/>
-      <c r="R7" s="109" t="str">
+      <c r="Q7" s="163"/>
+      <c r="R7" s="161" t="str">
         <f>Critérios!C20</f>
         <v>Transições entre estados</v>
       </c>
-      <c r="S7" s="110"/>
-      <c r="T7" s="111"/>
-      <c r="U7" s="109" t="str">
+      <c r="S7" s="162"/>
+      <c r="T7" s="163"/>
+      <c r="U7" s="161" t="str">
         <f>Critérios!C23</f>
         <v>Tabela de símbolos</v>
       </c>
-      <c r="V7" s="110"/>
-      <c r="W7" s="111"/>
-      <c r="X7" s="109" t="str">
+      <c r="V7" s="162"/>
+      <c r="W7" s="163"/>
+      <c r="X7" s="161" t="str">
         <f>Critérios!C26</f>
         <v>Comentários</v>
       </c>
-      <c r="Y7" s="111"/>
-      <c r="Z7" s="120" t="str">
+      <c r="Y7" s="163"/>
+      <c r="Z7" s="172" t="str">
         <f>Critérios!C28</f>
         <v>Listagem da entrada e erros</v>
       </c>
-      <c r="AA7" s="121"/>
-      <c r="AB7" s="122"/>
-      <c r="AC7" s="120" t="str">
+      <c r="AA7" s="173"/>
+      <c r="AB7" s="174"/>
+      <c r="AC7" s="172" t="str">
         <f>Critérios!C31</f>
         <v>Lista de tokens reconhecidos</v>
       </c>
-      <c r="AD7" s="121"/>
-      <c r="AE7" s="122"/>
-      <c r="AF7" s="120" t="str">
+      <c r="AD7" s="173"/>
+      <c r="AE7" s="174"/>
+      <c r="AF7" s="172" t="str">
         <f>Critérios!C34</f>
         <v>Tabela de símbolos</v>
       </c>
-      <c r="AG7" s="121"/>
-      <c r="AH7" s="122"/>
+      <c r="AG7" s="173"/>
+      <c r="AH7" s="174"/>
     </row>
     <row r="8" spans="1:34" s="47" customFormat="1" ht="3.75" customHeight="1">
       <c r="A8" s="61"/>
@@ -3946,8 +3946,8 @@
       <c r="AG8" s="70"/>
       <c r="AH8" s="71"/>
     </row>
-    <row r="9" spans="1:34" s="60" customFormat="1" ht="17" customHeight="1">
-      <c r="A9" s="124" t="s">
+    <row r="9" spans="1:34" s="60" customFormat="1" ht="16.95" customHeight="1">
+      <c r="A9" s="176" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="72"/>
@@ -4047,7 +4047,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" s="60" customFormat="1" ht="24" customHeight="1">
-      <c r="A10" s="125"/>
+      <c r="A10" s="177"/>
       <c r="B10" s="76" t="s">
         <v>63</v>
       </c>
@@ -4199,52 +4199,32 @@
       <c r="I12" s="89"/>
       <c r="J12" s="89"/>
       <c r="K12" s="89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="90"/>
-      <c r="N12" s="90">
-        <v>1</v>
-      </c>
-      <c r="O12" s="90">
-        <v>1</v>
-      </c>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
       <c r="P12" s="90"/>
-      <c r="Q12" s="90">
-        <v>1</v>
-      </c>
+      <c r="Q12" s="90"/>
       <c r="R12" s="90"/>
       <c r="S12" s="90"/>
       <c r="T12" s="90"/>
       <c r="U12" s="90"/>
-      <c r="V12" s="90">
-        <v>1</v>
-      </c>
-      <c r="W12" s="90">
-        <v>2</v>
-      </c>
+      <c r="V12" s="90"/>
+      <c r="W12" s="90"/>
       <c r="X12" s="90"/>
       <c r="Y12" s="90"/>
       <c r="Z12" s="91"/>
-      <c r="AA12" s="91">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="91">
-        <v>1</v>
-      </c>
+      <c r="AA12" s="91"/>
+      <c r="AB12" s="91"/>
       <c r="AC12" s="91"/>
-      <c r="AD12" s="91">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="91">
-        <v>1</v>
-      </c>
+      <c r="AD12" s="91"/>
+      <c r="AE12" s="91"/>
       <c r="AF12" s="91"/>
-      <c r="AG12" s="91">
-        <v>1</v>
-      </c>
+      <c r="AG12" s="91"/>
       <c r="AH12" s="92"/>
     </row>
     <row r="13" spans="1:34" s="87" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4263,52 +4243,32 @@
       <c r="I13" s="94"/>
       <c r="J13" s="94"/>
       <c r="K13" s="94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="95"/>
-      <c r="N13" s="95">
-        <v>1</v>
-      </c>
-      <c r="O13" s="95">
-        <v>1</v>
-      </c>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
       <c r="P13" s="95"/>
-      <c r="Q13" s="95">
-        <v>1</v>
-      </c>
+      <c r="Q13" s="95"/>
       <c r="R13" s="95"/>
       <c r="S13" s="95"/>
       <c r="T13" s="95"/>
       <c r="U13" s="95"/>
-      <c r="V13" s="95">
-        <v>1</v>
-      </c>
-      <c r="W13" s="95">
-        <v>2</v>
-      </c>
+      <c r="V13" s="95"/>
+      <c r="W13" s="95"/>
       <c r="X13" s="95"/>
       <c r="Y13" s="95"/>
       <c r="Z13" s="96"/>
-      <c r="AA13" s="96">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="96">
-        <v>1</v>
-      </c>
+      <c r="AA13" s="96"/>
+      <c r="AB13" s="96"/>
       <c r="AC13" s="96"/>
-      <c r="AD13" s="96">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="96">
-        <v>1</v>
-      </c>
+      <c r="AD13" s="96"/>
+      <c r="AE13" s="96"/>
       <c r="AF13" s="96"/>
-      <c r="AG13" s="96">
-        <v>1</v>
-      </c>
+      <c r="AG13" s="96"/>
       <c r="AH13" s="97"/>
     </row>
     <row r="14" spans="1:34" s="1" customFormat="1" ht="22.5" customHeight="1" thickTop="1">
@@ -4320,78 +4280,78 @@
       <c r="S14" s="11"/>
     </row>
     <row r="15" spans="1:34" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A15" s="123" t="s">
+      <c r="A15" s="175" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="123"/>
-      <c r="J15" s="123"/>
-      <c r="K15" s="123"/>
-      <c r="L15" s="123"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="123"/>
-      <c r="O15" s="123"/>
-      <c r="P15" s="123"/>
-      <c r="Q15" s="123"/>
-      <c r="R15" s="123"/>
-      <c r="S15" s="123"/>
-      <c r="T15" s="123"/>
-      <c r="U15" s="123"/>
-      <c r="V15" s="123"/>
-      <c r="W15" s="123"/>
-      <c r="X15" s="123"/>
-      <c r="Y15" s="123"/>
-      <c r="Z15" s="123"/>
-      <c r="AA15" s="123"/>
-      <c r="AB15" s="123"/>
-      <c r="AC15" s="123"/>
-      <c r="AD15" s="123"/>
-      <c r="AE15" s="123"/>
-      <c r="AF15" s="123"/>
-      <c r="AG15" s="123"/>
-      <c r="AH15" s="123"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="175"/>
+      <c r="F15" s="175"/>
+      <c r="G15" s="175"/>
+      <c r="H15" s="175"/>
+      <c r="I15" s="175"/>
+      <c r="J15" s="175"/>
+      <c r="K15" s="175"/>
+      <c r="L15" s="175"/>
+      <c r="M15" s="175"/>
+      <c r="N15" s="175"/>
+      <c r="O15" s="175"/>
+      <c r="P15" s="175"/>
+      <c r="Q15" s="175"/>
+      <c r="R15" s="175"/>
+      <c r="S15" s="175"/>
+      <c r="T15" s="175"/>
+      <c r="U15" s="175"/>
+      <c r="V15" s="175"/>
+      <c r="W15" s="175"/>
+      <c r="X15" s="175"/>
+      <c r="Y15" s="175"/>
+      <c r="Z15" s="175"/>
+      <c r="AA15" s="175"/>
+      <c r="AB15" s="175"/>
+      <c r="AC15" s="175"/>
+      <c r="AD15" s="175"/>
+      <c r="AE15" s="175"/>
+      <c r="AF15" s="175"/>
+      <c r="AG15" s="175"/>
+      <c r="AH15" s="175"/>
     </row>
     <row r="16" spans="1:34" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A16" s="123"/>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="123"/>
-      <c r="K16" s="123"/>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
-      <c r="P16" s="123"/>
-      <c r="Q16" s="123"/>
-      <c r="R16" s="123"/>
-      <c r="S16" s="123"/>
-      <c r="T16" s="123"/>
-      <c r="U16" s="123"/>
-      <c r="V16" s="123"/>
-      <c r="W16" s="123"/>
-      <c r="X16" s="123"/>
-      <c r="Y16" s="123"/>
-      <c r="Z16" s="123"/>
-      <c r="AA16" s="123"/>
-      <c r="AB16" s="123"/>
-      <c r="AC16" s="123"/>
-      <c r="AD16" s="123"/>
-      <c r="AE16" s="123"/>
-      <c r="AF16" s="123"/>
-      <c r="AG16" s="123"/>
-      <c r="AH16" s="123"/>
+      <c r="A16" s="175"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
+      <c r="O16" s="175"/>
+      <c r="P16" s="175"/>
+      <c r="Q16" s="175"/>
+      <c r="R16" s="175"/>
+      <c r="S16" s="175"/>
+      <c r="T16" s="175"/>
+      <c r="U16" s="175"/>
+      <c r="V16" s="175"/>
+      <c r="W16" s="175"/>
+      <c r="X16" s="175"/>
+      <c r="Y16" s="175"/>
+      <c r="Z16" s="175"/>
+      <c r="AA16" s="175"/>
+      <c r="AB16" s="175"/>
+      <c r="AC16" s="175"/>
+      <c r="AD16" s="175"/>
+      <c r="AE16" s="175"/>
+      <c r="AF16" s="175"/>
+      <c r="AG16" s="175"/>
+      <c r="AH16" s="175"/>
     </row>
   </sheetData>
   <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -4442,119 +4402,119 @@
   </sheetPr>
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.81640625" style="2" customWidth="1"/>
-    <col min="4" max="13" width="4.54296875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="0.81640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="7.36328125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="0.81640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="5.26953125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="0.81640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="7.36328125" style="11" customWidth="1"/>
-    <col min="20" max="20" width="0.81640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="5.26953125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="0.81640625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="7.36328125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="0.81640625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="5.26953125" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="0.77734375" style="2" customWidth="1"/>
+    <col min="4" max="13" width="4.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="0.77734375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="0.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="5.21875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="0.77734375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" style="11" customWidth="1"/>
+    <col min="20" max="20" width="0.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.21875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="0.77734375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="7.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="0.77734375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="5.21875" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="31">
-      <c r="A1" s="143" t="str">
+    <row r="1" spans="1:25" ht="31.2">
+      <c r="A1" s="198" t="str">
         <f>Critérios!A1:F1</f>
         <v>Compiladores - 2017.2</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
-      <c r="P1" s="144"/>
-      <c r="Q1" s="144"/>
-      <c r="R1" s="144"/>
-      <c r="S1" s="144"/>
-      <c r="T1" s="144"/>
-      <c r="U1" s="144"/>
-      <c r="V1" s="144"/>
-      <c r="W1" s="144"/>
-      <c r="X1" s="144"/>
-      <c r="Y1" s="145"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
+      <c r="Q1" s="199"/>
+      <c r="R1" s="199"/>
+      <c r="S1" s="199"/>
+      <c r="T1" s="199"/>
+      <c r="U1" s="199"/>
+      <c r="V1" s="199"/>
+      <c r="W1" s="199"/>
+      <c r="X1" s="199"/>
+      <c r="Y1" s="200"/>
     </row>
     <row r="2" spans="1:25" ht="26.25" customHeight="1">
-      <c r="A2" s="146" t="str">
+      <c r="A2" s="201" t="str">
         <f>Critérios!A2:F2</f>
         <v xml:space="preserve">Curso: Ciência da Computação </v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="148"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="202"/>
+      <c r="S2" s="202"/>
+      <c r="T2" s="202"/>
+      <c r="U2" s="202"/>
+      <c r="V2" s="202"/>
+      <c r="W2" s="202"/>
+      <c r="X2" s="202"/>
+      <c r="Y2" s="203"/>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="149" t="s">
+      <c r="A3" s="204" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
-      <c r="K3" s="150"/>
-      <c r="L3" s="150"/>
-      <c r="M3" s="150"/>
-      <c r="N3" s="150"/>
-      <c r="O3" s="150"/>
-      <c r="P3" s="150"/>
-      <c r="Q3" s="150"/>
-      <c r="R3" s="150"/>
-      <c r="S3" s="150"/>
-      <c r="T3" s="150"/>
-      <c r="U3" s="150"/>
-      <c r="V3" s="150"/>
-      <c r="W3" s="150"/>
-      <c r="X3" s="150"/>
-      <c r="Y3" s="151"/>
+      <c r="B3" s="205"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="205"/>
+      <c r="F3" s="205"/>
+      <c r="G3" s="205"/>
+      <c r="H3" s="205"/>
+      <c r="I3" s="205"/>
+      <c r="J3" s="205"/>
+      <c r="K3" s="205"/>
+      <c r="L3" s="205"/>
+      <c r="M3" s="205"/>
+      <c r="N3" s="205"/>
+      <c r="O3" s="205"/>
+      <c r="P3" s="205"/>
+      <c r="Q3" s="205"/>
+      <c r="R3" s="205"/>
+      <c r="S3" s="205"/>
+      <c r="T3" s="205"/>
+      <c r="U3" s="205"/>
+      <c r="V3" s="205"/>
+      <c r="W3" s="205"/>
+      <c r="X3" s="205"/>
+      <c r="Y3" s="206"/>
     </row>
     <row r="4" spans="1:25" ht="18" customHeight="1">
       <c r="A4" s="3"/>
@@ -4562,50 +4522,50 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="157"/>
-      <c r="G4" s="157"/>
-      <c r="H4" s="157"/>
-      <c r="I4" s="157"/>
-      <c r="J4" s="157"/>
-      <c r="K4" s="157"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-      <c r="N4" s="157"/>
-      <c r="O4" s="157"/>
+      <c r="F4" s="212"/>
+      <c r="G4" s="212"/>
+      <c r="H4" s="212"/>
+      <c r="I4" s="212"/>
+      <c r="J4" s="212"/>
+      <c r="K4" s="212"/>
+      <c r="L4" s="212"/>
+      <c r="M4" s="212"/>
+      <c r="N4" s="212"/>
+      <c r="O4" s="212"/>
       <c r="R4" s="42"/>
       <c r="S4" s="42"/>
     </row>
     <row r="5" spans="1:25" s="14" customFormat="1" ht="17.25" customHeight="1">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="D5" s="158" t="s">
+      <c r="D5" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
-      <c r="G5" s="158"/>
-      <c r="H5" s="158"/>
-      <c r="I5" s="158"/>
-      <c r="J5" s="158"/>
-      <c r="K5" s="158"/>
-      <c r="L5" s="158"/>
-      <c r="M5" s="158"/>
+      <c r="E5" s="213"/>
+      <c r="F5" s="213"/>
+      <c r="G5" s="213"/>
+      <c r="H5" s="213"/>
+      <c r="I5" s="213"/>
+      <c r="J5" s="213"/>
+      <c r="K5" s="213"/>
+      <c r="L5" s="213"/>
+      <c r="M5" s="213"/>
       <c r="O5" s="17"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="154" t="s">
+      <c r="Q5" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="S5" s="152" t="s">
+      <c r="S5" s="207" t="s">
         <v>56</v>
       </c>
       <c r="T5" s="1"/>
-      <c r="U5" s="154" t="s">
+      <c r="U5" s="209" t="s">
         <v>59</v>
       </c>
-      <c r="W5" s="141" t="s">
+      <c r="W5" s="196" t="s">
         <v>57</v>
       </c>
-      <c r="Y5" s="141" t="s">
+      <c r="Y5" s="196" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4614,43 +4574,43 @@
       <c r="B6" s="12"/>
       <c r="O6" s="17"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="155"/>
-      <c r="S6" s="153"/>
+      <c r="Q6" s="210"/>
+      <c r="S6" s="208"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="155"/>
-      <c r="W6" s="142"/>
-      <c r="Y6" s="142"/>
+      <c r="U6" s="210"/>
+      <c r="W6" s="197"/>
+      <c r="Y6" s="197"/>
     </row>
     <row r="7" spans="1:25" ht="21" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="156" t="s">
+      <c r="D7" s="211" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="156"/>
-      <c r="F7" s="159" t="str">
+      <c r="E7" s="211"/>
+      <c r="F7" s="214" t="str">
         <f>Erros!M5</f>
         <v>Implementação</v>
       </c>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
-      <c r="K7" s="160" t="str">
+      <c r="G7" s="214"/>
+      <c r="H7" s="214"/>
+      <c r="I7" s="214"/>
+      <c r="J7" s="214"/>
+      <c r="K7" s="215" t="str">
         <f>Erros!Z5</f>
         <v>Saídas</v>
       </c>
-      <c r="L7" s="160"/>
-      <c r="M7" s="160"/>
+      <c r="L7" s="215"/>
+      <c r="M7" s="215"/>
       <c r="N7" s="8"/>
       <c r="O7" s="17"/>
-      <c r="Q7" s="155"/>
+      <c r="Q7" s="210"/>
       <c r="R7" s="8"/>
-      <c r="S7" s="153"/>
-      <c r="U7" s="155"/>
-      <c r="W7" s="142"/>
-      <c r="Y7" s="142"/>
+      <c r="S7" s="208"/>
+      <c r="U7" s="210"/>
+      <c r="W7" s="197"/>
+      <c r="Y7" s="197"/>
     </row>
     <row r="8" spans="1:25" s="2" customFormat="1" ht="4.5" customHeight="1">
       <c r="A8" s="12"/>
@@ -4668,12 +4628,12 @@
       <c r="M8" s="18"/>
       <c r="N8" s="8"/>
       <c r="O8" s="19"/>
-      <c r="Q8" s="155"/>
+      <c r="Q8" s="210"/>
       <c r="R8" s="8"/>
-      <c r="S8" s="153"/>
-      <c r="U8" s="155"/>
-      <c r="W8" s="142"/>
-      <c r="Y8" s="142"/>
+      <c r="S8" s="208"/>
+      <c r="U8" s="210"/>
+      <c r="W8" s="197"/>
+      <c r="Y8" s="197"/>
     </row>
     <row r="9" spans="1:25" ht="12.75" customHeight="1">
       <c r="A9" s="12"/>
@@ -4724,12 +4684,12 @@
         <f>SUM(D9:M9)</f>
         <v>31</v>
       </c>
-      <c r="Q9" s="155"/>
+      <c r="Q9" s="210"/>
       <c r="R9" s="8"/>
-      <c r="S9" s="153"/>
-      <c r="U9" s="155"/>
-      <c r="W9" s="142"/>
-      <c r="Y9" s="142"/>
+      <c r="S9" s="208"/>
+      <c r="U9" s="210"/>
+      <c r="W9" s="197"/>
+      <c r="Y9" s="197"/>
     </row>
     <row r="10" spans="1:25" s="2" customFormat="1" ht="4.5" customHeight="1">
       <c r="A10" s="3"/>
@@ -4747,90 +4707,90 @@
       <c r="M10" s="21"/>
       <c r="N10" s="8"/>
       <c r="O10" s="9"/>
-      <c r="Q10" s="155"/>
+      <c r="Q10" s="210"/>
       <c r="R10" s="8"/>
-      <c r="S10" s="153"/>
-      <c r="U10" s="155"/>
-      <c r="W10" s="142"/>
-      <c r="Y10" s="142"/>
+      <c r="S10" s="208"/>
+      <c r="U10" s="210"/>
+      <c r="W10" s="197"/>
+      <c r="Y10" s="197"/>
     </row>
     <row r="11" spans="1:25" s="6" customFormat="1" ht="105" customHeight="1">
       <c r="A11" s="13"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="133" t="s">
+      <c r="D11" s="188" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="133" t="s">
+      <c r="E11" s="188" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="137" t="s">
+      <c r="F11" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="137" t="s">
+      <c r="G11" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="137" t="s">
+      <c r="H11" s="192" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="137" t="s">
+      <c r="I11" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="137" t="s">
+      <c r="J11" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="135" t="s">
+      <c r="K11" s="190" t="s">
         <v>50</v>
       </c>
-      <c r="L11" s="135" t="s">
+      <c r="L11" s="190" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="135" t="s">
+      <c r="M11" s="190" t="s">
         <v>6</v>
       </c>
       <c r="N11" s="5"/>
-      <c r="O11" s="161" t="s">
+      <c r="O11" s="216" t="s">
         <v>56</v>
       </c>
-      <c r="Q11" s="155"/>
+      <c r="Q11" s="210"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="153" t="s">
+      <c r="S11" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="U11" s="155"/>
-      <c r="W11" s="142"/>
-      <c r="Y11" s="142"/>
-    </row>
-    <row r="12" spans="1:25" s="6" customFormat="1" ht="30.65" customHeight="1">
-      <c r="A12" s="131" t="s">
+      <c r="U11" s="210"/>
+      <c r="W11" s="197"/>
+      <c r="Y11" s="197"/>
+    </row>
+    <row r="12" spans="1:25" s="6" customFormat="1" ht="30.6" customHeight="1">
+      <c r="A12" s="186" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="194" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="138"/>
-      <c r="J12" s="138"/>
-      <c r="K12" s="136"/>
-      <c r="L12" s="136"/>
-      <c r="M12" s="136"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="193"/>
+      <c r="I12" s="193"/>
+      <c r="J12" s="193"/>
+      <c r="K12" s="191"/>
+      <c r="L12" s="191"/>
+      <c r="M12" s="191"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="162"/>
-      <c r="Q12" s="155"/>
+      <c r="O12" s="217"/>
+      <c r="Q12" s="210"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="153"/>
-      <c r="U12" s="155"/>
-      <c r="W12" s="142"/>
-      <c r="Y12" s="142"/>
+      <c r="S12" s="208"/>
+      <c r="U12" s="210"/>
+      <c r="W12" s="197"/>
+      <c r="Y12" s="197"/>
     </row>
     <row r="13" spans="1:25" s="2" customFormat="1" ht="3" customHeight="1">
-      <c r="A13" s="132"/>
-      <c r="B13" s="140"/>
+      <c r="A13" s="187"/>
+      <c r="B13" s="195"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -4882,15 +4842,15 @@
       </c>
       <c r="E15" s="25">
         <f t="array" ref="E15">MAX(0,10-SUM(Erros!H$10:'Erros'!L$10*Erros!H12:'Erros'!L12))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F15" s="30">
         <f t="array" ref="F15">MAX(0,10-SUM(Erros!M$10:'Erros'!O$10*Erros!M12:'Erros'!O12))</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G15" s="30">
         <f t="array" ref="G15">MAX(0,10-SUM(Erros!P$10:'Erros'!Q$10*Erros!P12:'Erros'!Q12))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H15" s="30">
         <f t="array" ref="H15">MAX(0,10-SUM(Erros!R$10:'Erros'!T$10*Erros!R12:'Erros'!T12))</f>
@@ -4898,7 +4858,7 @@
       </c>
       <c r="I15" s="30">
         <f t="array" ref="I15">MAX(0,10-SUM(Erros!U$10:'Erros'!W$10*Erros!U12:'Erros'!W12))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J15" s="30">
         <f t="array" ref="J15">MAX(0,10-SUM(Erros!X$10:'Erros'!Y$10*Erros!X12:'Erros'!Y12))</f>
@@ -4906,39 +4866,39 @@
       </c>
       <c r="K15" s="31">
         <f t="array" ref="K15">MAX(0,10-SUM(Erros!Z$10:'Erros'!AB$10*Erros!Z12:'Erros'!AB12))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L15" s="31">
         <f t="array" ref="L15">MAX(0,10-SUM(Erros!AC$10:'Erros'!AE$10*Erros!AC12:'Erros'!AE12))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M15" s="31">
         <f t="array" ref="M15">MAX(0,10-SUM(Erros!AF$10:'Erros'!AH$10*Erros!AF12:'Erros'!AH12))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N15" s="23"/>
       <c r="O15" s="99">
         <f t="array" ref="O15">SUM(D$9:M$9*D15:M15)/O$9</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q15" s="45">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R15" s="23"/>
       <c r="S15" s="99">
         <f>IF(ISBLANK(Q15),O15,O15*(1-Q15))</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="U15" s="45">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="W15" s="98">
         <f>MAX(0,MIN(10,S15*U15*2))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Y15" s="43">
         <f>INT(10*W15+0.5)/10</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:25" s="10" customFormat="1" ht="13.5" customHeight="1" thickTop="1" thickBot="1">
@@ -4957,15 +4917,15 @@
       </c>
       <c r="E16" s="25">
         <f t="array" ref="E16">MAX(0,10-SUM(Erros!H$10:'Erros'!L$10*Erros!H13:'Erros'!L13))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F16" s="30">
         <f t="array" ref="F16">MAX(0,10-SUM(Erros!M$10:'Erros'!O$10*Erros!M13:'Erros'!O13))</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G16" s="30">
         <f t="array" ref="G16">MAX(0,10-SUM(Erros!P$10:'Erros'!Q$10*Erros!P13:'Erros'!Q13))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H16" s="30">
         <f t="array" ref="H16">MAX(0,10-SUM(Erros!R$10:'Erros'!T$10*Erros!R13:'Erros'!T13))</f>
@@ -4973,7 +4933,7 @@
       </c>
       <c r="I16" s="30">
         <f t="array" ref="I16">MAX(0,10-SUM(Erros!U$10:'Erros'!W$10*Erros!U13:'Erros'!W13))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J16" s="30">
         <f t="array" ref="J16">MAX(0,10-SUM(Erros!X$10:'Erros'!Y$10*Erros!X13:'Erros'!Y13))</f>
@@ -4981,98 +4941,98 @@
       </c>
       <c r="K16" s="31">
         <f t="array" ref="K16">MAX(0,10-SUM(Erros!Z$10:'Erros'!AB$10*Erros!Z13:'Erros'!AB13))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L16" s="31">
         <f t="array" ref="L16">MAX(0,10-SUM(Erros!AC$10:'Erros'!AE$10*Erros!AC13:'Erros'!AE13))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M16" s="31">
         <f t="array" ref="M16">MAX(0,10-SUM(Erros!AF$10:'Erros'!AH$10*Erros!AF13:'Erros'!AH13))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="99">
         <f t="array" ref="O16">SUM(D$9:M$9*D16:M16)/O$9</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q16" s="45">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R16" s="23"/>
       <c r="S16" s="99">
         <f t="shared" ref="S16" si="0">IF(ISBLANK(Q16),O16,O16*(1-Q16))</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="U16" s="44">
         <f>1-U15</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W16" s="98">
         <f>MAX(0,MIN(10,S16*U16*2))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="Y16" s="43">
         <f t="shared" ref="Y16" si="1">INT(10*W16+0.5)/10</f>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="22.5" customHeight="1" thickTop="1"/>
     <row r="18" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A18" s="123" t="s">
+      <c r="A18" s="175" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
-      <c r="K18" s="123"/>
-      <c r="L18" s="123"/>
-      <c r="M18" s="123"/>
-      <c r="N18" s="123"/>
-      <c r="O18" s="123"/>
-      <c r="P18" s="123"/>
-      <c r="Q18" s="123"/>
-      <c r="R18" s="123"/>
-      <c r="S18" s="123"/>
-      <c r="T18" s="123"/>
-      <c r="U18" s="123"/>
-      <c r="V18" s="123"/>
-      <c r="W18" s="123"/>
-      <c r="X18" s="123"/>
-      <c r="Y18" s="123"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="175"/>
+      <c r="D18" s="175"/>
+      <c r="E18" s="175"/>
+      <c r="F18" s="175"/>
+      <c r="G18" s="175"/>
+      <c r="H18" s="175"/>
+      <c r="I18" s="175"/>
+      <c r="J18" s="175"/>
+      <c r="K18" s="175"/>
+      <c r="L18" s="175"/>
+      <c r="M18" s="175"/>
+      <c r="N18" s="175"/>
+      <c r="O18" s="175"/>
+      <c r="P18" s="175"/>
+      <c r="Q18" s="175"/>
+      <c r="R18" s="175"/>
+      <c r="S18" s="175"/>
+      <c r="T18" s="175"/>
+      <c r="U18" s="175"/>
+      <c r="V18" s="175"/>
+      <c r="W18" s="175"/>
+      <c r="X18" s="175"/>
+      <c r="Y18" s="175"/>
     </row>
     <row r="19" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A19" s="123"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="123"/>
-      <c r="J19" s="123"/>
-      <c r="K19" s="123"/>
-      <c r="L19" s="123"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="123"/>
-      <c r="O19" s="123"/>
-      <c r="P19" s="123"/>
-      <c r="Q19" s="123"/>
-      <c r="R19" s="123"/>
-      <c r="S19" s="123"/>
-      <c r="T19" s="123"/>
-      <c r="U19" s="123"/>
-      <c r="V19" s="123"/>
-      <c r="W19" s="123"/>
-      <c r="X19" s="123"/>
-      <c r="Y19" s="123"/>
+      <c r="A19" s="175"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="175"/>
+      <c r="F19" s="175"/>
+      <c r="G19" s="175"/>
+      <c r="H19" s="175"/>
+      <c r="I19" s="175"/>
+      <c r="J19" s="175"/>
+      <c r="K19" s="175"/>
+      <c r="L19" s="175"/>
+      <c r="M19" s="175"/>
+      <c r="N19" s="175"/>
+      <c r="O19" s="175"/>
+      <c r="P19" s="175"/>
+      <c r="Q19" s="175"/>
+      <c r="R19" s="175"/>
+      <c r="S19" s="175"/>
+      <c r="T19" s="175"/>
+      <c r="U19" s="175"/>
+      <c r="V19" s="175"/>
+      <c r="W19" s="175"/>
+      <c r="X19" s="175"/>
+      <c r="Y19" s="175"/>
     </row>
   </sheetData>
   <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>

</xml_diff>